<commit_message>
ADD RTS and ITS incident reporting
</commit_message>
<xml_diff>
--- a/tools/dora/RTS/ITS-incident-reporting.xlsx
+++ b/tools/dora/RTS/ITS-incident-reporting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imanabshirali/Desktop/stage MAi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4765606-9A04-6C48-B68F-8EB61DC7DCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23018480-4F9E-5F4C-B195-2B3CFA3D3622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15020" activeTab="1" xr2:uid="{518DBCAF-BD91-AD48-90BD-EF4D4F6B9903}"/>
+    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15020" xr2:uid="{518DBCAF-BD91-AD48-90BD-EF4D4F6B9903}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="116">
   <si>
     <t>library_urn</t>
   </si>
@@ -110,15 +110,6 @@
   </si>
   <si>
     <t>Standard form for reporting of ICT-related major incidents</t>
-  </si>
-  <si>
-    <t>1.a</t>
-  </si>
-  <si>
-    <t>1.b</t>
-  </si>
-  <si>
-    <t>1.c</t>
   </si>
   <si>
     <t>Article 2</t>
@@ -380,13 +371,25 @@
 https://www.eiopa.europa.eu/document/download/0dfbccfd-97b2-4076-9644-b5cf4566fc6f_en?filename=JC%202024-33%20-%20Final%20report%20on%20the%20draft%20RTS%20and%20ITS%20on%20incident%20reporting.pdf</t>
   </si>
   <si>
-    <t>ESMA</t>
-  </si>
-  <si>
     <t>Financial entities shall ensure that the information contained in the cyber threat notification is complete and accurate.</t>
   </si>
   <si>
     <t>This Regulation shall be binding in its entirety and directly applicable in all Member States.</t>
+  </si>
+  <si>
+    <t>ITS DORA incident reporting</t>
+  </si>
+  <si>
+    <t>1.1.a</t>
+  </si>
+  <si>
+    <t>1.1.b</t>
+  </si>
+  <si>
+    <t>1.1.c</t>
+  </si>
+  <si>
+    <t>ESA</t>
   </si>
 </sst>
 </file>
@@ -823,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5239910-752D-8F4E-A0B5-A84B1FD6051E}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -866,7 +869,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -875,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -884,7 +887,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -893,7 +896,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -902,7 +905,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -920,7 +923,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -929,7 +932,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -938,7 +941,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -947,7 +950,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -956,7 +959,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>16</v>
@@ -971,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDDA96C-55DE-9A49-BAA5-162C404A0094}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A11" zoomScale="83" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,10 +1012,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1020,10 +1023,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1031,10 +1034,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1042,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -1053,10 +1056,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1064,10 +1067,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1075,10 +1078,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1086,10 +1089,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1097,10 +1100,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1108,10 +1111,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1131,114 +1134,114 @@
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="10">
         <v>2</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" s="10">
         <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B15" s="10">
         <v>3</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" s="10">
         <v>3</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" s="10">
         <v>2</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B18" s="10">
         <v>2</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="10">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="10">
-        <v>2</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" s="10">
         <v>2</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1247,21 +1250,21 @@
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="10">
         <v>2</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1270,21 +1273,21 @@
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="11" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -1293,38 +1296,38 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B26" s="10">
         <v>2</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B27" s="10">
         <v>2</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1333,21 +1336,21 @@
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="404" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B29" s="10">
         <v>2</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1356,21 +1359,21 @@
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B31" s="10">
         <v>2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1379,136 +1382,136 @@
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B33" s="10">
         <v>2</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B34" s="14">
         <v>3</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B35" s="14">
         <v>3</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B36" s="14">
         <v>3</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B37" s="14">
         <v>3</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B38" s="14">
         <v>3</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B39" s="14">
         <v>3</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B40" s="14">
         <v>2</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B41" s="14">
         <v>2</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1517,38 +1520,38 @@
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B43" s="10">
         <v>2</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B44" s="10">
         <v>2</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1557,10 +1560,10 @@
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1568,7 +1571,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1576,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>